<commit_message>
Update test folder with tests for checks #9 and #2
</commit_message>
<xml_diff>
--- a/test/ipachecknomiss/test.xlsx
+++ b/test/ipachecknomiss/test.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\test\ipachecknomiss\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="4. no miss" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -84,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -119,14 +114,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -392,20 +379,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="30" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +421,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -447,6 +434,7 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
+      <c r="E2" s="0"/>
       <c r="F2" t="s">
         <v>8</v>
       </c>
@@ -460,8 +448,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" s="0">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -473,6 +461,7 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
+      <c r="E3" s="0"/>
       <c r="F3" t="s">
         <v>8</v>
       </c>
@@ -486,8 +475,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" s="0">
         <v>10</v>
       </c>
       <c r="B4" t="s">
@@ -499,6 +488,7 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
+      <c r="E4" s="0"/>
       <c r="F4" t="s">
         <v>8</v>
       </c>
@@ -512,8 +502,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" s="0">
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -525,6 +515,7 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="0"/>
       <c r="F5" t="s">
         <v>16</v>
       </c>
@@ -538,8 +529,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" s="0">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -551,6 +542,7 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6" s="0"/>
       <c r="F6" t="s">
         <v>9</v>
       </c>

</xml_diff>